<commit_message>
Commeting the change -  implemented logger & Excel sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataOutsmart.xlsx
+++ b/src/test/resources/TestDataOutsmart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED729A7B-2B26-4190-84EE-FEB5957007A4}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D7E0221-7908-40C6-8772-C6F9993217FC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>FirstName</t>
   </si>
@@ -49,12 +49,40 @@
   </si>
   <si>
     <t>Bhavik@gmail.com</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>LoginCredentials</t>
+  </si>
+  <si>
+    <t>Sr No</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>bhavik.mohod@humancloud.co.in</t>
+  </si>
+  <si>
+    <t>Test@72809</t>
+  </si>
+  <si>
+    <t>Test@79856</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -72,15 +100,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -88,14 +122,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -431,51 +529,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.140625"/>
+    <col min="2" max="2" customWidth="true" width="36.0"/>
+    <col min="3" max="3" customWidth="true" width="20.0"/>
+    <col min="4" max="4" customWidth="true" width="31.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
         <v>7676565456</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="F6" t="s" s="0">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:C8"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{BD7E4E3E-0FF8-4BAE-82F9-9C367F481B69}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{DC2D6FFF-9F6E-4CBB-B27B-747CB954DB9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>